<commit_message>
Update card and item lists
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -557,7 +557,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F5" t="b">
@@ -817,7 +817,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F15" t="b">
@@ -921,7 +921,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F19" t="b">
@@ -947,7 +947,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F20" t="b">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F74" t="b">
@@ -2429,7 +2429,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F77" t="b">
@@ -2455,7 +2455,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F78" t="b">
@@ -2819,7 +2819,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F92" t="b">
@@ -3391,7 +3391,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F114" t="b">
@@ -3417,7 +3417,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F115" t="b">
@@ -3443,7 +3443,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F116" t="b">
@@ -3469,7 +3469,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F117" t="b">
@@ -3495,7 +3495,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F118" t="b">
@@ -3521,7 +3521,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F119" t="b">
@@ -3547,7 +3547,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F120" t="b">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F121" t="b">
@@ -3599,7 +3599,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F122" t="b">
@@ -3625,7 +3625,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F123" t="b">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F124" t="b">
@@ -3677,7 +3677,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F125" t="b">
@@ -4067,7 +4067,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F140" t="b">
@@ -4379,7 +4379,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F152" t="b">
@@ -4405,7 +4405,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F153" t="b">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F177" t="b">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F186" t="b">
@@ -5341,7 +5341,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F189" t="b">
@@ -5523,7 +5523,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F196" t="b">
@@ -5575,7 +5575,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F198" t="b">
@@ -6329,7 +6329,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F227" t="b">
@@ -7551,7 +7551,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F274" t="b">
@@ -7577,7 +7577,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F275" t="b">
@@ -7603,7 +7603,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F276" t="b">
@@ -7629,7 +7629,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F277" t="b">
@@ -7655,7 +7655,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F278" t="b">
@@ -7681,7 +7681,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F279" t="b">
@@ -7707,7 +7707,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F280" t="b">
@@ -7733,7 +7733,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F281" t="b">
@@ -7759,7 +7759,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F282" t="b">
@@ -7967,7 +7967,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F290" t="b">
@@ -8123,7 +8123,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F296" t="b">
@@ -8461,7 +8461,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F309" t="b">
@@ -8539,7 +8539,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F312" t="b">
@@ -8565,7 +8565,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F313" t="b">
@@ -8591,7 +8591,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F314" t="b">
@@ -8669,7 +8669,7 @@
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F317" t="b">
@@ -9241,7 +9241,7 @@
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F339" t="b">
@@ -9267,7 +9267,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F340" t="b">
@@ -10203,7 +10203,7 @@
       </c>
       <c r="E376" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F376" t="b">
@@ -10255,7 +10255,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F378" t="b">
@@ -10307,7 +10307,7 @@
       </c>
       <c r="E380" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F380" t="b">
@@ -10437,7 +10437,7 @@
       </c>
       <c r="E385" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F385" t="b">
@@ -10515,7 +10515,7 @@
       </c>
       <c r="E388" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F388" t="b">
@@ -10567,7 +10567,7 @@
       </c>
       <c r="E390" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F390" t="b">
@@ -10941,7 +10941,7 @@
       <c r="D407" t="inlineStr"/>
       <c r="E407" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F407" t="b">
@@ -11249,7 +11249,7 @@
       <c r="D421" t="inlineStr"/>
       <c r="E421" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F421" t="b">
@@ -11381,7 +11381,7 @@
       <c r="D427" t="inlineStr"/>
       <c r="E427" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F427" t="b">
@@ -11601,7 +11601,7 @@
       <c r="D437" t="inlineStr"/>
       <c r="E437" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F437" t="b">
@@ -12063,7 +12063,7 @@
       <c r="D458" t="inlineStr"/>
       <c r="E458" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F458" t="b">
@@ -12085,7 +12085,7 @@
       <c r="D459" t="inlineStr"/>
       <c r="E459" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F459" t="b">
@@ -12129,7 +12129,7 @@
       <c r="D461" t="inlineStr"/>
       <c r="E461" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F461" t="b">
@@ -12151,7 +12151,7 @@
       <c r="D462" t="inlineStr"/>
       <c r="E462" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F462" t="b">
@@ -12239,7 +12239,7 @@
       <c r="D466" t="inlineStr"/>
       <c r="E466" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F466" t="b">
@@ -12305,7 +12305,7 @@
       <c r="D469" t="inlineStr"/>
       <c r="E469" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F469" t="b">
@@ -12569,7 +12569,7 @@
       <c r="D481" t="inlineStr"/>
       <c r="E481" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F481" t="b">
@@ -12657,7 +12657,7 @@
       <c r="D485" t="inlineStr"/>
       <c r="E485" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F485" t="b">
@@ -12723,7 +12723,7 @@
       <c r="D488" t="inlineStr"/>
       <c r="E488" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F488" t="b">
@@ -12943,7 +12943,7 @@
       <c r="D498" t="inlineStr"/>
       <c r="E498" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F498" t="b">
@@ -13845,7 +13845,7 @@
       <c r="D539" t="inlineStr"/>
       <c r="E539" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F539" t="b">
@@ -13955,7 +13955,7 @@
       <c r="D544" t="inlineStr"/>
       <c r="E544" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F544" t="b">
@@ -14065,7 +14065,7 @@
       <c r="D549" t="inlineStr"/>
       <c r="E549" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F549" t="b">
@@ -14109,7 +14109,7 @@
       <c r="D551" t="inlineStr"/>
       <c r="E551" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F551" t="b">
@@ -14175,7 +14175,7 @@
       <c r="D554" t="inlineStr"/>
       <c r="E554" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F554" t="b">
@@ -14637,7 +14637,7 @@
       <c r="D575" t="inlineStr"/>
       <c r="E575" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F575" t="b">
@@ -14747,7 +14747,7 @@
       <c r="D580" t="inlineStr"/>
       <c r="E580" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F580" t="b">
@@ -14763,13 +14763,13 @@
       </c>
       <c r="C581" t="inlineStr">
         <is>
-          <t>Gishath, Sun's Avatar</t>
+          <t>Gisela, Blade of Goldnight</t>
         </is>
       </c>
       <c r="D581" t="inlineStr"/>
       <c r="E581" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F581" t="b">
@@ -14785,13 +14785,13 @@
       </c>
       <c r="C582" t="inlineStr">
         <is>
-          <t>Gix, Yawgmoth Praetor</t>
+          <t>Gishath, Sun's Avatar</t>
         </is>
       </c>
       <c r="D582" t="inlineStr"/>
       <c r="E582" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F582" t="b">
@@ -14807,13 +14807,13 @@
       </c>
       <c r="C583" t="inlineStr">
         <is>
-          <t>Glacial Fortress</t>
+          <t>Gix, Yawgmoth Praetor</t>
         </is>
       </c>
       <c r="D583" t="inlineStr"/>
       <c r="E583" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F583" t="b">
@@ -14829,13 +14829,13 @@
       </c>
       <c r="C584" t="inlineStr">
         <is>
-          <t>Goldspan Dragon</t>
+          <t>Glacial Fortress</t>
         </is>
       </c>
       <c r="D584" t="inlineStr"/>
       <c r="E584" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F584" t="b">
@@ -14851,13 +14851,13 @@
       </c>
       <c r="C585" t="inlineStr">
         <is>
-          <t>Goring Ceratops</t>
+          <t>Goldspan Dragon</t>
         </is>
       </c>
       <c r="D585" t="inlineStr"/>
       <c r="E585" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F585" t="b">
@@ -14873,13 +14873,13 @@
       </c>
       <c r="C586" t="inlineStr">
         <is>
-          <t>Goro-Goro and Satoru</t>
+          <t>Goring Ceratops</t>
         </is>
       </c>
       <c r="D586" t="inlineStr"/>
       <c r="E586" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F586" t="b">
@@ -14895,7 +14895,7 @@
       </c>
       <c r="C587" t="inlineStr">
         <is>
-          <t>Goro-Goro, Disciple of Ryusei</t>
+          <t>Goro-Goro and Satoru</t>
         </is>
       </c>
       <c r="D587" t="inlineStr"/>
@@ -14917,13 +14917,13 @@
       </c>
       <c r="C588" t="inlineStr">
         <is>
-          <t>Grand Warlord Radha</t>
+          <t>Goro-Goro, Disciple of Ryusei</t>
         </is>
       </c>
       <c r="D588" t="inlineStr"/>
       <c r="E588" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F588" t="b">
@@ -14939,13 +14939,13 @@
       </c>
       <c r="C589" t="inlineStr">
         <is>
-          <t>Graven Cairns</t>
+          <t>Grand Warlord Radha</t>
         </is>
       </c>
       <c r="D589" t="inlineStr"/>
       <c r="E589" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F589" t="b">
@@ -14961,13 +14961,13 @@
       </c>
       <c r="C590" t="inlineStr">
         <is>
-          <t>Grazilaxx, Illithid Scholar</t>
+          <t>Graven Cairns</t>
         </is>
       </c>
       <c r="D590" t="inlineStr"/>
       <c r="E590" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F590" t="b">
@@ -14983,7 +14983,7 @@
       </c>
       <c r="C591" t="inlineStr">
         <is>
-          <t>Grim Hireling</t>
+          <t>Grazilaxx, Illithid Scholar</t>
         </is>
       </c>
       <c r="D591" t="inlineStr"/>
@@ -15005,13 +15005,13 @@
       </c>
       <c r="C592" t="inlineStr">
         <is>
-          <t>Gruul Signet</t>
+          <t>Grim Hireling</t>
         </is>
       </c>
       <c r="D592" t="inlineStr"/>
       <c r="E592" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F592" t="b">
@@ -15027,13 +15027,13 @@
       </c>
       <c r="C593" t="inlineStr">
         <is>
-          <t>Guardian of Faith</t>
+          <t>Gruul Signet</t>
         </is>
       </c>
       <c r="D593" t="inlineStr"/>
       <c r="E593" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F593" t="b">
@@ -15049,13 +15049,13 @@
       </c>
       <c r="C594" t="inlineStr">
         <is>
-          <t>Guardian of Ghirapur</t>
+          <t>Guardian of Faith</t>
         </is>
       </c>
       <c r="D594" t="inlineStr"/>
       <c r="E594" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F594" t="b">
@@ -15071,13 +15071,13 @@
       </c>
       <c r="C595" t="inlineStr">
         <is>
-          <t>Guttersnipe</t>
+          <t>Guardian of Ghirapur</t>
         </is>
       </c>
       <c r="D595" t="inlineStr"/>
       <c r="E595" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F595" t="b">
@@ -15093,13 +15093,13 @@
       </c>
       <c r="C596" t="inlineStr">
         <is>
-          <t>Hallowed Fountain</t>
+          <t>Guttersnipe</t>
         </is>
       </c>
       <c r="D596" t="inlineStr"/>
       <c r="E596" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F596" t="b">
@@ -15115,13 +15115,13 @@
       </c>
       <c r="C597" t="inlineStr">
         <is>
-          <t>Halvar, God of Battle</t>
+          <t>Hallowed Fountain</t>
         </is>
       </c>
       <c r="D597" t="inlineStr"/>
       <c r="E597" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F597" t="b">
@@ -15137,13 +15137,13 @@
       </c>
       <c r="C598" t="inlineStr">
         <is>
-          <t>Hanweir Battlements</t>
+          <t>Halvar, God of Battle</t>
         </is>
       </c>
       <c r="D598" t="inlineStr"/>
       <c r="E598" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F598" t="b">
@@ -15159,13 +15159,13 @@
       </c>
       <c r="C599" t="inlineStr">
         <is>
-          <t>Harsh Mentor</t>
+          <t>Hanweir Battlements</t>
         </is>
       </c>
       <c r="D599" t="inlineStr"/>
       <c r="E599" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F599" t="b">
@@ -15181,13 +15181,13 @@
       </c>
       <c r="C600" t="inlineStr">
         <is>
-          <t>Harvest Season</t>
+          <t>Harsh Mentor</t>
         </is>
       </c>
       <c r="D600" t="inlineStr"/>
       <c r="E600" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F600" t="b">
@@ -15203,13 +15203,13 @@
       </c>
       <c r="C601" t="inlineStr">
         <is>
-          <t>Haunted Ridge</t>
+          <t>Harvest Season</t>
         </is>
       </c>
       <c r="D601" t="inlineStr"/>
       <c r="E601" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F601" t="b">
@@ -15225,13 +15225,13 @@
       </c>
       <c r="C602" t="inlineStr">
         <is>
-          <t>Hazardous Blast</t>
+          <t>Haunted Ridge</t>
         </is>
       </c>
       <c r="D602" t="inlineStr"/>
       <c r="E602" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F602" t="b">
@@ -15247,13 +15247,13 @@
       </c>
       <c r="C603" t="inlineStr">
         <is>
-          <t>Heartflame Duelist</t>
+          <t>Hazardous Blast</t>
         </is>
       </c>
       <c r="D603" t="inlineStr"/>
       <c r="E603" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F603" t="b">
@@ -15269,13 +15269,13 @@
       </c>
       <c r="C604" t="inlineStr">
         <is>
-          <t>Heartstone</t>
+          <t>Heartflame Duelist</t>
         </is>
       </c>
       <c r="D604" t="inlineStr"/>
       <c r="E604" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F604" t="b">
@@ -15291,7 +15291,7 @@
       </c>
       <c r="C605" t="inlineStr">
         <is>
-          <t>Hellish Rebuke</t>
+          <t>Heartstone</t>
         </is>
       </c>
       <c r="D605" t="inlineStr"/>
@@ -15313,13 +15313,13 @@
       </c>
       <c r="C606" t="inlineStr">
         <is>
-          <t>Hellrider</t>
+          <t>Hellish Rebuke</t>
         </is>
       </c>
       <c r="D606" t="inlineStr"/>
       <c r="E606" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F606" t="b">
@@ -15335,13 +15335,13 @@
       </c>
       <c r="C607" t="inlineStr">
         <is>
-          <t>Heroic Intervention</t>
+          <t>Hellrider</t>
         </is>
       </c>
       <c r="D607" t="inlineStr"/>
       <c r="E607" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F607" t="b">
@@ -15363,7 +15363,7 @@
       <c r="D608" t="inlineStr"/>
       <c r="E608" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F608" t="b">
@@ -15379,13 +15379,13 @@
       </c>
       <c r="C609" t="inlineStr">
         <is>
-          <t>High Alert</t>
+          <t>Heroic Intervention</t>
         </is>
       </c>
       <c r="D609" t="inlineStr"/>
       <c r="E609" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F609" t="b">
@@ -15401,13 +15401,13 @@
       </c>
       <c r="C610" t="inlineStr">
         <is>
-          <t>Hinterland Harbor</t>
+          <t>High Alert</t>
         </is>
       </c>
       <c r="D610" t="inlineStr"/>
       <c r="E610" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F610" t="b">
@@ -15423,13 +15423,13 @@
       </c>
       <c r="C611" t="inlineStr">
         <is>
-          <t>Horn of the Mark</t>
+          <t>Hinterland Harbor</t>
         </is>
       </c>
       <c r="D611" t="inlineStr"/>
       <c r="E611" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F611" t="b">
@@ -15445,13 +15445,13 @@
       </c>
       <c r="C612" t="inlineStr">
         <is>
-          <t>Hour of Devastation</t>
+          <t>Horn of the Mark</t>
         </is>
       </c>
       <c r="D612" t="inlineStr"/>
       <c r="E612" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F612" t="b">
@@ -15467,13 +15467,13 @@
       </c>
       <c r="C613" t="inlineStr">
         <is>
-          <t>Hour of Reckoning</t>
+          <t>Hour of Devastation</t>
         </is>
       </c>
       <c r="D613" t="inlineStr"/>
       <c r="E613" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F613" t="b">
@@ -15489,13 +15489,13 @@
       </c>
       <c r="C614" t="inlineStr">
         <is>
-          <t>Hover Barrier</t>
+          <t>Hour of Reckoning</t>
         </is>
       </c>
       <c r="D614" t="inlineStr"/>
       <c r="E614" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F614" t="b">
@@ -15511,13 +15511,13 @@
       </c>
       <c r="C615" t="inlineStr">
         <is>
-          <t>Huatli, Radiant Champion</t>
+          <t>Hover Barrier</t>
         </is>
       </c>
       <c r="D615" t="inlineStr"/>
       <c r="E615" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F615" t="b">
@@ -15533,13 +15533,13 @@
       </c>
       <c r="C616" t="inlineStr">
         <is>
-          <t>Huatli, Warrior Poet</t>
+          <t>Huatli, Radiant Champion</t>
         </is>
       </c>
       <c r="D616" t="inlineStr"/>
       <c r="E616" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F616" t="b">
@@ -15555,13 +15555,13 @@
       </c>
       <c r="C617" t="inlineStr">
         <is>
-          <t>Hurloon Battle Hymn</t>
+          <t>Huatli, Warrior Poet</t>
         </is>
       </c>
       <c r="D617" t="inlineStr"/>
       <c r="E617" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F617" t="b">
@@ -15577,13 +15577,13 @@
       </c>
       <c r="C618" t="inlineStr">
         <is>
-          <t>Idol of Oblivion</t>
+          <t>Hurloon Battle Hymn</t>
         </is>
       </c>
       <c r="D618" t="inlineStr"/>
       <c r="E618" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F618" t="b">
@@ -15599,13 +15599,13 @@
       </c>
       <c r="C619" t="inlineStr">
         <is>
-          <t>Imodane's Recruiter</t>
+          <t>Idol of Oblivion</t>
         </is>
       </c>
       <c r="D619" t="inlineStr"/>
       <c r="E619" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F619" t="b">
@@ -15737,7 +15737,7 @@
       <c r="D625" t="inlineStr"/>
       <c r="E625" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F625" t="b">
@@ -16397,7 +16397,7 @@
       <c r="D655" t="inlineStr"/>
       <c r="E655" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F655" t="b">
@@ -16441,7 +16441,7 @@
       <c r="D657" t="inlineStr"/>
       <c r="E657" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F657" t="b">
@@ -16661,7 +16661,7 @@
       <c r="D667" t="inlineStr"/>
       <c r="E667" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F667" t="b">
@@ -17365,7 +17365,7 @@
       <c r="D699" t="inlineStr"/>
       <c r="E699" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F699" t="b">
@@ -17541,7 +17541,7 @@
       <c r="D707" t="inlineStr"/>
       <c r="E707" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F707" t="b">
@@ -17651,7 +17651,7 @@
       <c r="D712" t="inlineStr"/>
       <c r="E712" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F712" t="b">
@@ -18289,7 +18289,7 @@
       <c r="D741" t="inlineStr"/>
       <c r="E741" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F741" t="b">
@@ -18399,7 +18399,7 @@
       <c r="D746" t="inlineStr"/>
       <c r="E746" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F746" t="b">
@@ -18525,13 +18525,13 @@
       </c>
       <c r="C752" t="inlineStr">
         <is>
-          <t>OlÃ³rin's Searing Light</t>
+          <t>Ominous Seas</t>
         </is>
       </c>
       <c r="D752" t="inlineStr"/>
       <c r="E752" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F752" t="b">
@@ -18547,13 +18547,13 @@
       </c>
       <c r="C753" t="inlineStr">
         <is>
-          <t>Ominous Seas</t>
+          <t>Orthion, Hero of Lavabrink</t>
         </is>
       </c>
       <c r="D753" t="inlineStr"/>
       <c r="E753" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F753" t="b">
@@ -18569,13 +18569,13 @@
       </c>
       <c r="C754" t="inlineStr">
         <is>
-          <t>Orthion, Hero of Lavabrink</t>
+          <t>Otepec Huntmaster</t>
         </is>
       </c>
       <c r="D754" t="inlineStr"/>
       <c r="E754" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F754" t="b">
@@ -18591,13 +18591,13 @@
       </c>
       <c r="C755" t="inlineStr">
         <is>
-          <t>Otepec Huntmaster</t>
+          <t>Overgrown Battlement</t>
         </is>
       </c>
       <c r="D755" t="inlineStr"/>
       <c r="E755" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F755" t="b">
@@ -18613,7 +18613,7 @@
       </c>
       <c r="C756" t="inlineStr">
         <is>
-          <t>Overgrown Battlement</t>
+          <t>Overgrown Farmland</t>
         </is>
       </c>
       <c r="D756" t="inlineStr"/>
@@ -18635,13 +18635,13 @@
       </c>
       <c r="C757" t="inlineStr">
         <is>
-          <t>Overgrown Farmland</t>
+          <t>Overwhelming Stampede</t>
         </is>
       </c>
       <c r="D757" t="inlineStr"/>
       <c r="E757" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F757" t="b">
@@ -18657,13 +18657,13 @@
       </c>
       <c r="C758" t="inlineStr">
         <is>
-          <t>Overwhelming Stampede</t>
+          <t>Parasitic Impetus</t>
         </is>
       </c>
       <c r="D758" t="inlineStr"/>
       <c r="E758" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F758" t="b">
@@ -18679,13 +18679,13 @@
       </c>
       <c r="C759" t="inlineStr">
         <is>
-          <t>Parasitic Impetus</t>
+          <t>Path of Ancestry</t>
         </is>
       </c>
       <c r="D759" t="inlineStr"/>
       <c r="E759" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F759" t="b">
@@ -18701,7 +18701,7 @@
       </c>
       <c r="C760" t="inlineStr">
         <is>
-          <t>Path of Ancestry</t>
+          <t>Path to Exile</t>
         </is>
       </c>
       <c r="D760" t="inlineStr"/>
@@ -18729,7 +18729,7 @@
       <c r="D761" t="inlineStr"/>
       <c r="E761" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F761" t="b">
@@ -18751,7 +18751,7 @@
       <c r="D762" t="inlineStr"/>
       <c r="E762" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F762" t="b">
@@ -18767,13 +18767,13 @@
       </c>
       <c r="C763" t="inlineStr">
         <is>
-          <t>Path to Exile</t>
+          <t>Pathbreaker Ibex</t>
         </is>
       </c>
       <c r="D763" t="inlineStr"/>
       <c r="E763" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F763" t="b">
@@ -18789,13 +18789,13 @@
       </c>
       <c r="C764" t="inlineStr">
         <is>
-          <t>Pathbreaker Ibex</t>
+          <t>Pemmin's Aura</t>
         </is>
       </c>
       <c r="D764" t="inlineStr"/>
       <c r="E764" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F764" t="b">
@@ -18811,13 +18811,13 @@
       </c>
       <c r="C765" t="inlineStr">
         <is>
-          <t>Pemmin's Aura</t>
+          <t>Perimeter Captain</t>
         </is>
       </c>
       <c r="D765" t="inlineStr"/>
       <c r="E765" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F765" t="b">
@@ -18833,13 +18833,13 @@
       </c>
       <c r="C766" t="inlineStr">
         <is>
-          <t>Perimeter Captain</t>
+          <t>Phoenix Chick</t>
         </is>
       </c>
       <c r="D766" t="inlineStr"/>
       <c r="E766" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F766" t="b">
@@ -18855,13 +18855,13 @@
       </c>
       <c r="C767" t="inlineStr">
         <is>
-          <t>Phoenix Chick</t>
+          <t>Polyraptor</t>
         </is>
       </c>
       <c r="D767" t="inlineStr"/>
       <c r="E767" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F767" t="b">
@@ -18877,13 +18877,13 @@
       </c>
       <c r="C768" t="inlineStr">
         <is>
-          <t>Polyraptor</t>
+          <t>Prairie Stream</t>
         </is>
       </c>
       <c r="D768" t="inlineStr"/>
       <c r="E768" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F768" t="b">
@@ -18899,13 +18899,13 @@
       </c>
       <c r="C769" t="inlineStr">
         <is>
-          <t>Prairie Stream</t>
+          <t>Prava of the Steel Legion</t>
         </is>
       </c>
       <c r="D769" t="inlineStr"/>
       <c r="E769" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F769" t="b">
@@ -18921,13 +18921,13 @@
       </c>
       <c r="C770" t="inlineStr">
         <is>
-          <t>Prava of the Steel Legion</t>
+          <t>Price of Progress</t>
         </is>
       </c>
       <c r="D770" t="inlineStr"/>
       <c r="E770" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F770" t="b">
@@ -18943,7 +18943,7 @@
       </c>
       <c r="C771" t="inlineStr">
         <is>
-          <t>Price of Progress</t>
+          <t>Primal Amulet</t>
         </is>
       </c>
       <c r="D771" t="inlineStr"/>
@@ -18965,13 +18965,13 @@
       </c>
       <c r="C772" t="inlineStr">
         <is>
-          <t>Primal Amulet</t>
+          <t>Prime Speaker Zegana</t>
         </is>
       </c>
       <c r="D772" t="inlineStr"/>
       <c r="E772" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F772" t="b">
@@ -18987,13 +18987,13 @@
       </c>
       <c r="C773" t="inlineStr">
         <is>
-          <t>Prime Speaker Zegana</t>
+          <t>Professional Face-Breaker</t>
         </is>
       </c>
       <c r="D773" t="inlineStr"/>
       <c r="E773" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F773" t="b">
@@ -19009,7 +19009,7 @@
       </c>
       <c r="C774" t="inlineStr">
         <is>
-          <t>Professional Face-Breaker</t>
+          <t>Prosperous Thief</t>
         </is>
       </c>
       <c r="D774" t="inlineStr"/>
@@ -19031,13 +19031,13 @@
       </c>
       <c r="C775" t="inlineStr">
         <is>
-          <t>Prosperous Thief</t>
+          <t>Puresteel Paladin</t>
         </is>
       </c>
       <c r="D775" t="inlineStr"/>
       <c r="E775" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F775" t="b">
@@ -19053,13 +19053,13 @@
       </c>
       <c r="C776" t="inlineStr">
         <is>
-          <t>Puresteel Paladin</t>
+          <t>Pyromancer's Goggles</t>
         </is>
       </c>
       <c r="D776" t="inlineStr"/>
       <c r="E776" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F776" t="b">
@@ -19075,13 +19075,13 @@
       </c>
       <c r="C777" t="inlineStr">
         <is>
-          <t>Pyromancer's Goggles</t>
+          <t>Queen Allenal of Ruadach</t>
         </is>
       </c>
       <c r="D777" t="inlineStr"/>
       <c r="E777" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F777" t="b">
@@ -19097,13 +19097,13 @@
       </c>
       <c r="C778" t="inlineStr">
         <is>
-          <t>Queen Allenal of Ruadach</t>
+          <t>Quest for Ula's Temple</t>
         </is>
       </c>
       <c r="D778" t="inlineStr"/>
       <c r="E778" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F778" t="b">
@@ -19119,13 +19119,13 @@
       </c>
       <c r="C779" t="inlineStr">
         <is>
-          <t>Quest for Ula's Temple</t>
+          <t>Quick Study</t>
         </is>
       </c>
       <c r="D779" t="inlineStr"/>
       <c r="E779" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F779" t="b">
@@ -19147,7 +19147,7 @@
       <c r="D780" t="inlineStr"/>
       <c r="E780" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F780" t="b">
@@ -19163,13 +19163,13 @@
       </c>
       <c r="C781" t="inlineStr">
         <is>
-          <t>Quick Study</t>
+          <t>Quintorius, Loremaster</t>
         </is>
       </c>
       <c r="D781" t="inlineStr"/>
       <c r="E781" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F781" t="b">
@@ -19185,13 +19185,13 @@
       </c>
       <c r="C782" t="inlineStr">
         <is>
-          <t>Quintorius, Loremaster</t>
+          <t>Radha, Heir to Keld</t>
         </is>
       </c>
       <c r="D782" t="inlineStr"/>
       <c r="E782" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F782" t="b">
@@ -19207,13 +19207,13 @@
       </c>
       <c r="C783" t="inlineStr">
         <is>
-          <t>Radha, Heir to Keld</t>
+          <t>Radiant Scrollwielder</t>
         </is>
       </c>
       <c r="D783" t="inlineStr"/>
       <c r="E783" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F783" t="b">
@@ -19229,13 +19229,13 @@
       </c>
       <c r="C784" t="inlineStr">
         <is>
-          <t>Radiant Scrollwielder</t>
+          <t>Raging Swordtooth</t>
         </is>
       </c>
       <c r="D784" t="inlineStr"/>
       <c r="E784" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F784" t="b">
@@ -19251,13 +19251,13 @@
       </c>
       <c r="C785" t="inlineStr">
         <is>
-          <t>Raging Swordtooth</t>
+          <t>Rakdos Signet</t>
         </is>
       </c>
       <c r="D785" t="inlineStr"/>
       <c r="E785" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F785" t="b">
@@ -19273,13 +19273,13 @@
       </c>
       <c r="C786" t="inlineStr">
         <is>
-          <t>Rakdos Signet</t>
+          <t>Rammas Echor, Ancient Shield</t>
         </is>
       </c>
       <c r="D786" t="inlineStr"/>
       <c r="E786" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F786" t="b">
@@ -19295,13 +19295,13 @@
       </c>
       <c r="C787" t="inlineStr">
         <is>
-          <t>Rammas Echor, Ancient Shield</t>
+          <t>Rampant Growth</t>
         </is>
       </c>
       <c r="D787" t="inlineStr"/>
       <c r="E787" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F787" t="b">
@@ -19323,7 +19323,7 @@
       <c r="D788" t="inlineStr"/>
       <c r="E788" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F788" t="b">
@@ -19339,13 +19339,13 @@
       </c>
       <c r="C789" t="inlineStr">
         <is>
-          <t>Rampant Growth</t>
+          <t>Ramunap Excavator</t>
         </is>
       </c>
       <c r="D789" t="inlineStr"/>
       <c r="E789" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F789" t="b">
@@ -19361,13 +19361,13 @@
       </c>
       <c r="C790" t="inlineStr">
         <is>
-          <t>Ramunap Excavator</t>
+          <t>Ranging Raptors</t>
         </is>
       </c>
       <c r="D790" t="inlineStr"/>
       <c r="E790" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F790" t="b">
@@ -19383,13 +19383,13 @@
       </c>
       <c r="C791" t="inlineStr">
         <is>
-          <t>Ranging Raptors</t>
+          <t>Reanimate</t>
         </is>
       </c>
       <c r="D791" t="inlineStr"/>
       <c r="E791" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F791" t="b">
@@ -19405,13 +19405,13 @@
       </c>
       <c r="C792" t="inlineStr">
         <is>
-          <t>Reanimate</t>
+          <t>Reconnaissance Mission</t>
         </is>
       </c>
       <c r="D792" t="inlineStr"/>
       <c r="E792" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F792" t="b">
@@ -19427,13 +19427,13 @@
       </c>
       <c r="C793" t="inlineStr">
         <is>
-          <t>Reconnaissance Mission</t>
+          <t>Regisaur Alpha</t>
         </is>
       </c>
       <c r="D793" t="inlineStr"/>
       <c r="E793" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F793" t="b">
@@ -19449,13 +19449,13 @@
       </c>
       <c r="C794" t="inlineStr">
         <is>
-          <t>Regisaur Alpha</t>
+          <t>Reinforced Ronin</t>
         </is>
       </c>
       <c r="D794" t="inlineStr"/>
       <c r="E794" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F794" t="b">
@@ -19471,13 +19471,13 @@
       </c>
       <c r="C795" t="inlineStr">
         <is>
-          <t>Reinforced Ronin</t>
+          <t>Rejuvenating Springs</t>
         </is>
       </c>
       <c r="D795" t="inlineStr"/>
       <c r="E795" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F795" t="b">
@@ -19493,13 +19493,13 @@
       </c>
       <c r="C796" t="inlineStr">
         <is>
-          <t>Rejuvenating Springs</t>
+          <t>Relentless Assault</t>
         </is>
       </c>
       <c r="D796" t="inlineStr"/>
       <c r="E796" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F796" t="b">
@@ -19515,13 +19515,13 @@
       </c>
       <c r="C797" t="inlineStr">
         <is>
-          <t>Relentless Assault</t>
+          <t>Reliquary Tower</t>
         </is>
       </c>
       <c r="D797" t="inlineStr"/>
       <c r="E797" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F797" t="b">
@@ -19543,7 +19543,7 @@
       <c r="D798" t="inlineStr"/>
       <c r="E798" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F798" t="b">
@@ -19559,13 +19559,13 @@
       </c>
       <c r="C799" t="inlineStr">
         <is>
-          <t>Reliquary Tower</t>
+          <t>Rem Karolus, Stalwart Slayer</t>
         </is>
       </c>
       <c r="D799" t="inlineStr"/>
       <c r="E799" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F799" t="b">
@@ -19587,7 +19587,7 @@
       <c r="D800" t="inlineStr"/>
       <c r="E800" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F800" t="b">
@@ -19603,13 +19603,13 @@
       </c>
       <c r="C801" t="inlineStr">
         <is>
-          <t>Rem Karolus, Stalwart Slayer</t>
+          <t>Restless Vinestalk</t>
         </is>
       </c>
       <c r="D801" t="inlineStr"/>
       <c r="E801" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F801" t="b">
@@ -19625,13 +19625,13 @@
       </c>
       <c r="C802" t="inlineStr">
         <is>
-          <t>Restless Vinestalk</t>
+          <t>Restoration Angel</t>
         </is>
       </c>
       <c r="D802" t="inlineStr"/>
       <c r="E802" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F802" t="b">
@@ -19647,13 +19647,13 @@
       </c>
       <c r="C803" t="inlineStr">
         <is>
-          <t>Restoration Angel</t>
+          <t>Return of the Wildspeaker</t>
         </is>
       </c>
       <c r="D803" t="inlineStr"/>
       <c r="E803" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F803" t="b">
@@ -19669,13 +19669,13 @@
       </c>
       <c r="C804" t="inlineStr">
         <is>
-          <t>Return of the Wildspeaker</t>
+          <t>Reverberate</t>
         </is>
       </c>
       <c r="D804" t="inlineStr"/>
       <c r="E804" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F804" t="b">
@@ -19691,7 +19691,7 @@
       </c>
       <c r="C805" t="inlineStr">
         <is>
-          <t>Reverberate</t>
+          <t>Revitalize</t>
         </is>
       </c>
       <c r="D805" t="inlineStr"/>
@@ -19713,13 +19713,13 @@
       </c>
       <c r="C806" t="inlineStr">
         <is>
-          <t>Revitalize</t>
+          <t>Rhythm of the Wild</t>
         </is>
       </c>
       <c r="D806" t="inlineStr"/>
       <c r="E806" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F806" t="b">
@@ -19735,13 +19735,13 @@
       </c>
       <c r="C807" t="inlineStr">
         <is>
-          <t>Rhythm of the Wild</t>
+          <t>Rip Apart</t>
         </is>
       </c>
       <c r="D807" t="inlineStr"/>
       <c r="E807" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F807" t="b">
@@ -19757,13 +19757,13 @@
       </c>
       <c r="C808" t="inlineStr">
         <is>
-          <t>Rip Apart</t>
+          <t>Ripjaw Raptor</t>
         </is>
       </c>
       <c r="D808" t="inlineStr"/>
       <c r="E808" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F808" t="b">
@@ -19779,13 +19779,13 @@
       </c>
       <c r="C809" t="inlineStr">
         <is>
-          <t>Ripjaw Raptor</t>
+          <t>Riptide Turtle</t>
         </is>
       </c>
       <c r="D809" t="inlineStr"/>
       <c r="E809" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F809" t="b">
@@ -19801,13 +19801,13 @@
       </c>
       <c r="C810" t="inlineStr">
         <is>
-          <t>Riptide Turtle</t>
+          <t>Rishkar's Expertise</t>
         </is>
       </c>
       <c r="D810" t="inlineStr"/>
       <c r="E810" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F810" t="b">
@@ -19823,13 +19823,13 @@
       </c>
       <c r="C811" t="inlineStr">
         <is>
-          <t>Rishkar's Expertise</t>
+          <t>Rising of the Day</t>
         </is>
       </c>
       <c r="D811" t="inlineStr"/>
       <c r="E811" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F811" t="b">
@@ -19851,7 +19851,7 @@
       <c r="D812" t="inlineStr"/>
       <c r="E812" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F812" t="b">
@@ -19873,7 +19873,7 @@
       <c r="D813" t="inlineStr"/>
       <c r="E813" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F813" t="b">
@@ -19889,13 +19889,13 @@
       </c>
       <c r="C814" t="inlineStr">
         <is>
-          <t>Rising of the Day</t>
+          <t>Rockfall Vale</t>
         </is>
       </c>
       <c r="D814" t="inlineStr"/>
       <c r="E814" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F814" t="b">
@@ -19917,7 +19917,7 @@
       <c r="D815" t="inlineStr"/>
       <c r="E815" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F815" t="b">
@@ -19933,13 +19933,13 @@
       </c>
       <c r="C816" t="inlineStr">
         <is>
-          <t>Rockfall Vale</t>
+          <t>Rogue's Passage</t>
         </is>
       </c>
       <c r="D816" t="inlineStr"/>
       <c r="E816" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F816" t="b">
@@ -19961,7 +19961,7 @@
       <c r="D817" t="inlineStr"/>
       <c r="E817" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F817" t="b">
@@ -19983,7 +19983,7 @@
       <c r="D818" t="inlineStr"/>
       <c r="E818" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F818" t="b">
@@ -20005,7 +20005,7 @@
       <c r="D819" t="inlineStr"/>
       <c r="E819" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F819" t="b">
@@ -20021,13 +20021,13 @@
       </c>
       <c r="C820" t="inlineStr">
         <is>
-          <t>Rogue's Passage</t>
+          <t>Roiling Regrowth</t>
         </is>
       </c>
       <c r="D820" t="inlineStr"/>
       <c r="E820" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F820" t="b">
@@ -20043,13 +20043,13 @@
       </c>
       <c r="C821" t="inlineStr">
         <is>
-          <t>Roiling Regrowth</t>
+          <t>Rolling Earthquake</t>
         </is>
       </c>
       <c r="D821" t="inlineStr"/>
       <c r="E821" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F821" t="b">
@@ -20065,13 +20065,13 @@
       </c>
       <c r="C822" t="inlineStr">
         <is>
-          <t>Rolling Earthquake</t>
+          <t>Rootborn Defenses</t>
         </is>
       </c>
       <c r="D822" t="inlineStr"/>
       <c r="E822" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F822" t="b">
@@ -20087,13 +20087,13 @@
       </c>
       <c r="C823" t="inlineStr">
         <is>
-          <t>Rootborn Defenses</t>
+          <t>Rootbound Crag</t>
         </is>
       </c>
       <c r="D823" t="inlineStr"/>
       <c r="E823" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F823" t="b">
@@ -20115,7 +20115,7 @@
       <c r="D824" t="inlineStr"/>
       <c r="E824" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F824" t="b">
@@ -20131,7 +20131,7 @@
       </c>
       <c r="C825" t="inlineStr">
         <is>
-          <t>Rootbound Crag</t>
+          <t>Ruby, Daring Tracker</t>
         </is>
       </c>
       <c r="D825" t="inlineStr"/>
@@ -20153,7 +20153,7 @@
       </c>
       <c r="C826" t="inlineStr">
         <is>
-          <t>Ruby, Daring Tracker</t>
+          <t>Rulik Mons, Warren Chief</t>
         </is>
       </c>
       <c r="D826" t="inlineStr"/>
@@ -20175,13 +20175,13 @@
       </c>
       <c r="C827" t="inlineStr">
         <is>
-          <t>Rulik Mons, Warren Chief</t>
+          <t>Rumor Gatherer</t>
         </is>
       </c>
       <c r="D827" t="inlineStr"/>
       <c r="E827" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F827" t="b">
@@ -20197,13 +20197,13 @@
       </c>
       <c r="C828" t="inlineStr">
         <is>
-          <t>Rumor Gatherer</t>
+          <t>Rune-Scarred Demon</t>
         </is>
       </c>
       <c r="D828" t="inlineStr"/>
       <c r="E828" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F828" t="b">
@@ -20219,13 +20219,13 @@
       </c>
       <c r="C829" t="inlineStr">
         <is>
-          <t>Rune-Scarred Demon</t>
+          <t>Runic Armasaur</t>
         </is>
       </c>
       <c r="D829" t="inlineStr"/>
       <c r="E829" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F829" t="b">
@@ -20241,13 +20241,13 @@
       </c>
       <c r="C830" t="inlineStr">
         <is>
-          <t>Runic Armasaur</t>
+          <t>Sacred Fire</t>
         </is>
       </c>
       <c r="D830" t="inlineStr"/>
       <c r="E830" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F830" t="b">
@@ -20263,13 +20263,13 @@
       </c>
       <c r="C831" t="inlineStr">
         <is>
-          <t>Sacred Fire</t>
+          <t>Sacred Foundry</t>
         </is>
       </c>
       <c r="D831" t="inlineStr"/>
       <c r="E831" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F831" t="b">
@@ -20291,7 +20291,7 @@
       <c r="D832" t="inlineStr"/>
       <c r="E832" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F832" t="b">
@@ -20307,13 +20307,13 @@
       </c>
       <c r="C833" t="inlineStr">
         <is>
-          <t>Sacred Foundry</t>
+          <t>Saheeli, the Sun's Brilliance</t>
         </is>
       </c>
       <c r="D833" t="inlineStr"/>
       <c r="E833" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F833" t="b">
@@ -20329,7 +20329,7 @@
       </c>
       <c r="C834" t="inlineStr">
         <is>
-          <t>Saheeli, the Sun's Brilliance</t>
+          <t>Satoru Umezawa</t>
         </is>
       </c>
       <c r="D834" t="inlineStr"/>
@@ -20351,13 +20351,13 @@
       </c>
       <c r="C835" t="inlineStr">
         <is>
-          <t>Satoru Umezawa</t>
+          <t>Savai Triome</t>
         </is>
       </c>
       <c r="D835" t="inlineStr"/>
       <c r="E835" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F835" t="b">
@@ -20373,13 +20373,13 @@
       </c>
       <c r="C836" t="inlineStr">
         <is>
-          <t>Savai Triome</t>
+          <t>Scourge of Fleets</t>
         </is>
       </c>
       <c r="D836" t="inlineStr"/>
       <c r="E836" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F836" t="b">
@@ -20395,13 +20395,13 @@
       </c>
       <c r="C837" t="inlineStr">
         <is>
-          <t>Scourge of Fleets</t>
+          <t>Seaside Citadel</t>
         </is>
       </c>
       <c r="D837" t="inlineStr"/>
       <c r="E837" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F837" t="b">
@@ -20417,13 +20417,13 @@
       </c>
       <c r="C838" t="inlineStr">
         <is>
-          <t>Seaside Citadel</t>
+          <t>Secluded Courtyard</t>
         </is>
       </c>
       <c r="D838" t="inlineStr"/>
       <c r="E838" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F838" t="b">
@@ -20439,13 +20439,13 @@
       </c>
       <c r="C839" t="inlineStr">
         <is>
-          <t>Secluded Courtyard</t>
+          <t>Shadowspear</t>
         </is>
       </c>
       <c r="D839" t="inlineStr"/>
       <c r="E839" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F839" t="b">
@@ -20461,13 +20461,13 @@
       </c>
       <c r="C840" t="inlineStr">
         <is>
-          <t>Shadowspear</t>
+          <t>Shattered Sanctum</t>
         </is>
       </c>
       <c r="D840" t="inlineStr"/>
       <c r="E840" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F840" t="b">
@@ -20483,13 +20483,13 @@
       </c>
       <c r="C841" t="inlineStr">
         <is>
-          <t>Shattered Sanctum</t>
+          <t>Shield Sphere</t>
         </is>
       </c>
       <c r="D841" t="inlineStr"/>
       <c r="E841" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F841" t="b">
@@ -20505,7 +20505,7 @@
       </c>
       <c r="C842" t="inlineStr">
         <is>
-          <t>Shield Sphere</t>
+          <t>Shield-Wall Sentinel</t>
         </is>
       </c>
       <c r="D842" t="inlineStr"/>
@@ -20527,13 +20527,13 @@
       </c>
       <c r="C843" t="inlineStr">
         <is>
-          <t>Shield-Wall Sentinel</t>
+          <t>Shipbreaker Kraken</t>
         </is>
       </c>
       <c r="D843" t="inlineStr"/>
       <c r="E843" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F843" t="b">
@@ -20549,13 +20549,13 @@
       </c>
       <c r="C844" t="inlineStr">
         <is>
-          <t>Shipbreaker Kraken</t>
+          <t>Sigarda's Aid</t>
         </is>
       </c>
       <c r="D844" t="inlineStr"/>
       <c r="E844" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F844" t="b">
@@ -20571,7 +20571,7 @@
       </c>
       <c r="C845" t="inlineStr">
         <is>
-          <t>Sigarda's Aid</t>
+          <t>Sigiled Sword of Valeron</t>
         </is>
       </c>
       <c r="D845" t="inlineStr"/>
@@ -20593,13 +20593,13 @@
       </c>
       <c r="C846" t="inlineStr">
         <is>
-          <t>Sigiled Sword of Valeron</t>
+          <t>Silent-Blade Oni</t>
         </is>
       </c>
       <c r="D846" t="inlineStr"/>
       <c r="E846" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F846" t="b">
@@ -20615,7 +20615,7 @@
       </c>
       <c r="C847" t="inlineStr">
         <is>
-          <t>Silent-Blade Oni</t>
+          <t>Silver-Fur Master</t>
         </is>
       </c>
       <c r="D847" t="inlineStr"/>
@@ -20637,13 +20637,13 @@
       </c>
       <c r="C848" t="inlineStr">
         <is>
-          <t>Silver-Fur Master</t>
+          <t>Silverclad Ferocidons</t>
         </is>
       </c>
       <c r="D848" t="inlineStr"/>
       <c r="E848" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F848" t="b">
@@ -20659,13 +20659,13 @@
       </c>
       <c r="C849" t="inlineStr">
         <is>
-          <t>Silverclad Ferocidons</t>
+          <t>Simic Sky Swallower</t>
         </is>
       </c>
       <c r="D849" t="inlineStr"/>
       <c r="E849" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F849" t="b">
@@ -20681,13 +20681,13 @@
       </c>
       <c r="C850" t="inlineStr">
         <is>
-          <t>Simic Sky Swallower</t>
+          <t>Single Combat</t>
         </is>
       </c>
       <c r="D850" t="inlineStr"/>
       <c r="E850" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F850" t="b">
@@ -20703,13 +20703,13 @@
       </c>
       <c r="C851" t="inlineStr">
         <is>
-          <t>Single Combat</t>
+          <t>Slaughter the Strong</t>
         </is>
       </c>
       <c r="D851" t="inlineStr"/>
       <c r="E851" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F851" t="b">
@@ -20725,13 +20725,13 @@
       </c>
       <c r="C852" t="inlineStr">
         <is>
-          <t>Slaughter the Strong</t>
+          <t>Slinn Voda, the Rising Deep</t>
         </is>
       </c>
       <c r="D852" t="inlineStr"/>
       <c r="E852" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F852" t="b">
@@ -20747,13 +20747,13 @@
       </c>
       <c r="C853" t="inlineStr">
         <is>
-          <t>Slinn Voda, the Rising Deep</t>
+          <t>Slither Blade</t>
         </is>
       </c>
       <c r="D853" t="inlineStr"/>
       <c r="E853" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F853" t="b">
@@ -20769,13 +20769,13 @@
       </c>
       <c r="C854" t="inlineStr">
         <is>
-          <t>Slither Blade</t>
+          <t>Sol Ring</t>
         </is>
       </c>
       <c r="D854" t="inlineStr"/>
       <c r="E854" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F854" t="b">
@@ -20797,7 +20797,7 @@
       <c r="D855" t="inlineStr"/>
       <c r="E855" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F855" t="b">
@@ -20819,7 +20819,7 @@
       <c r="D856" t="inlineStr"/>
       <c r="E856" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F856" t="b">
@@ -20835,13 +20835,13 @@
       </c>
       <c r="C857" t="inlineStr">
         <is>
-          <t>Sol Ring</t>
+          <t>Solphim, Mayhem Dominus</t>
         </is>
       </c>
       <c r="D857" t="inlineStr"/>
       <c r="E857" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F857" t="b">
@@ -20857,13 +20857,13 @@
       </c>
       <c r="C858" t="inlineStr">
         <is>
-          <t>Solphim, Mayhem Dominus</t>
+          <t>Song of Totentanz</t>
         </is>
       </c>
       <c r="D858" t="inlineStr"/>
       <c r="E858" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F858" t="b">
@@ -20879,13 +20879,13 @@
       </c>
       <c r="C859" t="inlineStr">
         <is>
-          <t>Song of Totentanz</t>
+          <t>Sower of Discord</t>
         </is>
       </c>
       <c r="D859" t="inlineStr"/>
       <c r="E859" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F859" t="b">
@@ -20901,13 +20901,13 @@
       </c>
       <c r="C860" t="inlineStr">
         <is>
-          <t>Sower of Discord</t>
+          <t>Spara's Headquarters</t>
         </is>
       </c>
       <c r="D860" t="inlineStr"/>
       <c r="E860" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F860" t="b">
@@ -20923,13 +20923,13 @@
       </c>
       <c r="C861" t="inlineStr">
         <is>
-          <t>Spara's Headquarters</t>
+          <t>Spectator Seating</t>
         </is>
       </c>
       <c r="D861" t="inlineStr"/>
       <c r="E861" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F861" t="b">
@@ -20951,7 +20951,7 @@
       <c r="D862" t="inlineStr"/>
       <c r="E862" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F862" t="b">
@@ -20967,13 +20967,13 @@
       </c>
       <c r="C863" t="inlineStr">
         <is>
-          <t>Spectator Seating</t>
+          <t>Spire Garden</t>
         </is>
       </c>
       <c r="D863" t="inlineStr"/>
       <c r="E863" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F863" t="b">
@@ -20989,13 +20989,13 @@
       </c>
       <c r="C864" t="inlineStr">
         <is>
-          <t>Spire Garden</t>
+          <t>Sram, Senior Edificer</t>
         </is>
       </c>
       <c r="D864" t="inlineStr"/>
       <c r="E864" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F864" t="b">
@@ -21011,13 +21011,13 @@
       </c>
       <c r="C865" t="inlineStr">
         <is>
-          <t>Sram, Senior Edificer</t>
+          <t>Stalwart Shield-Bearers</t>
         </is>
       </c>
       <c r="D865" t="inlineStr"/>
       <c r="E865" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F865" t="b">
@@ -21033,13 +21033,13 @@
       </c>
       <c r="C866" t="inlineStr">
         <is>
-          <t>Stalwart Shield-Bearers</t>
+          <t>Star of Extinction</t>
         </is>
       </c>
       <c r="D866" t="inlineStr"/>
       <c r="E866" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F866" t="b">
@@ -21055,7 +21055,7 @@
       </c>
       <c r="C867" t="inlineStr">
         <is>
-          <t>Star of Extinction</t>
+          <t>Starstorm</t>
         </is>
       </c>
       <c r="D867" t="inlineStr"/>
@@ -21077,13 +21077,13 @@
       </c>
       <c r="C868" t="inlineStr">
         <is>
-          <t>Starstorm</t>
+          <t>Steelshaper's Gift</t>
         </is>
       </c>
       <c r="D868" t="inlineStr"/>
       <c r="E868" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F868" t="b">
@@ -21099,13 +21099,13 @@
       </c>
       <c r="C869" t="inlineStr">
         <is>
-          <t>Steelshaper's Gift</t>
+          <t>Stomping Ground</t>
         </is>
       </c>
       <c r="D869" t="inlineStr"/>
       <c r="E869" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F869" t="b">
@@ -21127,7 +21127,7 @@
       <c r="D870" t="inlineStr"/>
       <c r="E870" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F870" t="b">
@@ -21143,13 +21143,13 @@
       </c>
       <c r="C871" t="inlineStr">
         <is>
-          <t>Stomping Ground</t>
+          <t>Stoneskin</t>
         </is>
       </c>
       <c r="D871" t="inlineStr"/>
       <c r="E871" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F871" t="b">
@@ -21165,13 +21165,13 @@
       </c>
       <c r="C872" t="inlineStr">
         <is>
-          <t>Stoneskin</t>
+          <t>Storm's Wrath</t>
         </is>
       </c>
       <c r="D872" t="inlineStr"/>
       <c r="E872" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F872" t="b">
@@ -21187,13 +21187,13 @@
       </c>
       <c r="C873" t="inlineStr">
         <is>
-          <t>Storm's Wrath</t>
+          <t>Stormsurge Kraken</t>
         </is>
       </c>
       <c r="D873" t="inlineStr"/>
       <c r="E873" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F873" t="b">
@@ -21209,7 +21209,7 @@
       </c>
       <c r="C874" t="inlineStr">
         <is>
-          <t>Stormsurge Kraken</t>
+          <t>Stormtide Leviathan</t>
         </is>
       </c>
       <c r="D874" t="inlineStr"/>
@@ -21231,13 +21231,13 @@
       </c>
       <c r="C875" t="inlineStr">
         <is>
-          <t>Stormtide Leviathan</t>
+          <t>Stroke of Midnight</t>
         </is>
       </c>
       <c r="D875" t="inlineStr"/>
       <c r="E875" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F875" t="b">
@@ -21259,7 +21259,7 @@
       <c r="D876" t="inlineStr"/>
       <c r="E876" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F876" t="b">
@@ -21275,13 +21275,13 @@
       </c>
       <c r="C877" t="inlineStr">
         <is>
-          <t>Stroke of Midnight</t>
+          <t>Stuffy Doll</t>
         </is>
       </c>
       <c r="D877" t="inlineStr"/>
       <c r="E877" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F877" t="b">
@@ -21303,7 +21303,7 @@
       <c r="D878" t="inlineStr"/>
       <c r="E878" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F878" t="b">
@@ -21319,7 +21319,7 @@
       </c>
       <c r="C879" t="inlineStr">
         <is>
-          <t>Stuffy Doll</t>
+          <t>Sudden Spoiling</t>
         </is>
       </c>
       <c r="D879" t="inlineStr"/>
@@ -21341,13 +21341,13 @@
       </c>
       <c r="C880" t="inlineStr">
         <is>
-          <t>Sudden Spoiling</t>
+          <t>Sundering Growth</t>
         </is>
       </c>
       <c r="D880" t="inlineStr"/>
       <c r="E880" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F880" t="b">
@@ -21363,13 +21363,13 @@
       </c>
       <c r="C881" t="inlineStr">
         <is>
-          <t>Sundering Growth</t>
+          <t>Sundown Pass</t>
         </is>
       </c>
       <c r="D881" t="inlineStr"/>
       <c r="E881" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F881" t="b">
@@ -21391,7 +21391,7 @@
       <c r="D882" t="inlineStr"/>
       <c r="E882" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F882" t="b">
@@ -21407,13 +21407,13 @@
       </c>
       <c r="C883" t="inlineStr">
         <is>
-          <t>Sundown Pass</t>
+          <t>Sunforger</t>
         </is>
       </c>
       <c r="D883" t="inlineStr"/>
       <c r="E883" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F883" t="b">
@@ -21429,13 +21429,13 @@
       </c>
       <c r="C884" t="inlineStr">
         <is>
-          <t>Sunforger</t>
+          <t>Sunpetal Grove</t>
         </is>
       </c>
       <c r="D884" t="inlineStr"/>
       <c r="E884" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F884" t="b">
@@ -21451,13 +21451,13 @@
       </c>
       <c r="C885" t="inlineStr">
         <is>
-          <t>Sunpetal Grove</t>
+          <t>Sunscape Familiar</t>
         </is>
       </c>
       <c r="D885" t="inlineStr"/>
       <c r="E885" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F885" t="b">
@@ -21473,13 +21473,13 @@
       </c>
       <c r="C886" t="inlineStr">
         <is>
-          <t>Sunscape Familiar</t>
+          <t>Swamp</t>
         </is>
       </c>
       <c r="D886" t="inlineStr"/>
       <c r="E886" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F886" t="b">
@@ -21539,13 +21539,13 @@
       </c>
       <c r="C889" t="inlineStr">
         <is>
-          <t>Swamp</t>
+          <t>Sword of Feast and Famine</t>
         </is>
       </c>
       <c r="D889" t="inlineStr"/>
       <c r="E889" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F889" t="b">
@@ -21561,7 +21561,7 @@
       </c>
       <c r="C890" t="inlineStr">
         <is>
-          <t>Sword of Feast and Famine</t>
+          <t>Sword of Hearth and Home</t>
         </is>
       </c>
       <c r="D890" t="inlineStr"/>
@@ -21583,7 +21583,7 @@
       </c>
       <c r="C891" t="inlineStr">
         <is>
-          <t>Sword of Hearth and Home</t>
+          <t>Sword of Vengeance</t>
         </is>
       </c>
       <c r="D891" t="inlineStr"/>
@@ -21605,13 +21605,13 @@
       </c>
       <c r="C892" t="inlineStr">
         <is>
-          <t>Sword of Vengeance</t>
+          <t>Sword of the Animist</t>
         </is>
       </c>
       <c r="D892" t="inlineStr"/>
       <c r="E892" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F892" t="b">
@@ -21627,13 +21627,13 @@
       </c>
       <c r="C893" t="inlineStr">
         <is>
-          <t>Sword of the Animist</t>
+          <t>Swords to Plowshares</t>
         </is>
       </c>
       <c r="D893" t="inlineStr"/>
       <c r="E893" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F893" t="b">
@@ -21655,7 +21655,7 @@
       <c r="D894" t="inlineStr"/>
       <c r="E894" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F894" t="b">
@@ -21671,13 +21671,13 @@
       </c>
       <c r="C895" t="inlineStr">
         <is>
-          <t>Swords to Plowshares</t>
+          <t>Sylvan Caryatid</t>
         </is>
       </c>
       <c r="D895" t="inlineStr"/>
       <c r="E895" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F895" t="b">
@@ -21693,13 +21693,13 @@
       </c>
       <c r="C896" t="inlineStr">
         <is>
-          <t>Sylvan Caryatid</t>
+          <t>Syr Gwyn, Hero of Ashvale</t>
         </is>
       </c>
       <c r="D896" t="inlineStr"/>
       <c r="E896" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F896" t="b">
@@ -21715,13 +21715,13 @@
       </c>
       <c r="C897" t="inlineStr">
         <is>
-          <t>Syr Gwyn, Hero of Ashvale</t>
+          <t>Talisman of Conviction</t>
         </is>
       </c>
       <c r="D897" t="inlineStr"/>
       <c r="E897" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F897" t="b">
@@ -21743,7 +21743,7 @@
       <c r="D898" t="inlineStr"/>
       <c r="E898" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F898" t="b">
@@ -21759,13 +21759,13 @@
       </c>
       <c r="C899" t="inlineStr">
         <is>
-          <t>Talisman of Conviction</t>
+          <t>Talisman of Curiosity</t>
         </is>
       </c>
       <c r="D899" t="inlineStr"/>
       <c r="E899" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F899" t="b">
@@ -21781,13 +21781,13 @@
       </c>
       <c r="C900" t="inlineStr">
         <is>
-          <t>Talisman of Curiosity</t>
+          <t>Talisman of Dominance</t>
         </is>
       </c>
       <c r="D900" t="inlineStr"/>
       <c r="E900" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F900" t="b">
@@ -21803,13 +21803,13 @@
       </c>
       <c r="C901" t="inlineStr">
         <is>
-          <t>Talisman of Dominance</t>
+          <t>Talisman of Hierarchy</t>
         </is>
       </c>
       <c r="D901" t="inlineStr"/>
       <c r="E901" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F901" t="b">
@@ -21825,7 +21825,7 @@
       </c>
       <c r="C902" t="inlineStr">
         <is>
-          <t>Talisman of Hierarchy</t>
+          <t>Talisman of Indulgence</t>
         </is>
       </c>
       <c r="D902" t="inlineStr"/>
@@ -21853,7 +21853,7 @@
       <c r="D903" t="inlineStr"/>
       <c r="E903" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F903" t="b">
@@ -21869,13 +21869,13 @@
       </c>
       <c r="C904" t="inlineStr">
         <is>
-          <t>Talisman of Indulgence</t>
+          <t>Tectonic Giant</t>
         </is>
       </c>
       <c r="D904" t="inlineStr"/>
       <c r="E904" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>wulfgar</t>
         </is>
       </c>
       <c r="F904" t="b">
@@ -21891,13 +21891,13 @@
       </c>
       <c r="C905" t="inlineStr">
         <is>
-          <t>Tectonic Giant</t>
+          <t>Teleportation Circle</t>
         </is>
       </c>
       <c r="D905" t="inlineStr"/>
       <c r="E905" t="inlineStr">
         <is>
-          <t>wulfgar</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F905" t="b">
@@ -21913,13 +21913,13 @@
       </c>
       <c r="C906" t="inlineStr">
         <is>
-          <t>Teleportation Circle</t>
+          <t>Temple Altisaur</t>
         </is>
       </c>
       <c r="D906" t="inlineStr"/>
       <c r="E906" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F906" t="b">
@@ -21935,7 +21935,7 @@
       </c>
       <c r="C907" t="inlineStr">
         <is>
-          <t>Temple Altisaur</t>
+          <t>Temple Garden</t>
         </is>
       </c>
       <c r="D907" t="inlineStr"/>
@@ -21963,7 +21963,7 @@
       <c r="D908" t="inlineStr"/>
       <c r="E908" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F908" t="b">
@@ -21979,13 +21979,13 @@
       </c>
       <c r="C909" t="inlineStr">
         <is>
-          <t>Temple Garden</t>
+          <t>Temple of Malice</t>
         </is>
       </c>
       <c r="D909" t="inlineStr"/>
       <c r="E909" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F909" t="b">
@@ -22001,13 +22001,13 @@
       </c>
       <c r="C910" t="inlineStr">
         <is>
-          <t>Temple of Malice</t>
+          <t>Temple of Silence</t>
         </is>
       </c>
       <c r="D910" t="inlineStr"/>
       <c r="E910" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F910" t="b">
@@ -22023,13 +22023,13 @@
       </c>
       <c r="C911" t="inlineStr">
         <is>
-          <t>Temple of Silence</t>
+          <t>Temple of Triumph</t>
         </is>
       </c>
       <c r="D911" t="inlineStr"/>
       <c r="E911" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>firesong</t>
         </is>
       </c>
       <c r="F911" t="b">
@@ -22051,7 +22051,7 @@
       <c r="D912" t="inlineStr"/>
       <c r="E912" t="inlineStr">
         <is>
-          <t>firesong</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F912" t="b">
@@ -22073,7 +22073,7 @@
       <c r="D913" t="inlineStr"/>
       <c r="E913" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F913" t="b">
@@ -22089,13 +22089,13 @@
       </c>
       <c r="C914" t="inlineStr">
         <is>
-          <t>Temple of Triumph</t>
+          <t>Terminate</t>
         </is>
       </c>
       <c r="D914" t="inlineStr"/>
       <c r="E914" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F914" t="b">
@@ -22117,7 +22117,7 @@
       <c r="D915" t="inlineStr"/>
       <c r="E915" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F915" t="b">
@@ -22133,13 +22133,13 @@
       </c>
       <c r="C916" t="inlineStr">
         <is>
-          <t>Terminate</t>
+          <t>Terror of the Peaks</t>
         </is>
       </c>
       <c r="D916" t="inlineStr"/>
       <c r="E916" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F916" t="b">
@@ -22155,13 +22155,13 @@
       </c>
       <c r="C917" t="inlineStr">
         <is>
-          <t>Terror of the Peaks</t>
+          <t>Tetsuko Umezawa, Fugitive</t>
         </is>
       </c>
       <c r="D917" t="inlineStr"/>
       <c r="E917" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F917" t="b">
@@ -22183,7 +22183,7 @@
       <c r="D918" t="inlineStr"/>
       <c r="E918" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F918" t="b">
@@ -22199,13 +22199,13 @@
       </c>
       <c r="C919" t="inlineStr">
         <is>
-          <t>Tetsuko Umezawa, Fugitive</t>
+          <t>Teyo, Geometric Tactician</t>
         </is>
       </c>
       <c r="D919" t="inlineStr"/>
       <c r="E919" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>arcades</t>
         </is>
       </c>
       <c r="F919" t="b">
@@ -22221,7 +22221,7 @@
       </c>
       <c r="C920" t="inlineStr">
         <is>
-          <t>Teyo, Geometric Tactician</t>
+          <t>The Birth of Meletis</t>
         </is>
       </c>
       <c r="D920" t="inlineStr"/>
@@ -22243,13 +22243,13 @@
       </c>
       <c r="C921" t="inlineStr">
         <is>
-          <t>The Birth of Meletis</t>
+          <t>The Circle of Loyalty</t>
         </is>
       </c>
       <c r="D921" t="inlineStr"/>
       <c r="E921" t="inlineStr">
         <is>
-          <t>arcades</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F921" t="b">
@@ -22265,13 +22265,13 @@
       </c>
       <c r="C922" t="inlineStr">
         <is>
-          <t>The Circle of Loyalty</t>
+          <t>The Eternal Wanderer</t>
         </is>
       </c>
       <c r="D922" t="inlineStr"/>
       <c r="E922" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>kaalia</t>
         </is>
       </c>
       <c r="F922" t="b">
@@ -22287,13 +22287,13 @@
       </c>
       <c r="C923" t="inlineStr">
         <is>
-          <t>The Eternal Wanderer</t>
+          <t>The Great Henge</t>
         </is>
       </c>
       <c r="D923" t="inlineStr"/>
       <c r="E923" t="inlineStr">
         <is>
-          <t>kaalia</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F923" t="b">
@@ -22309,13 +22309,13 @@
       </c>
       <c r="C924" t="inlineStr">
         <is>
-          <t>The Great Henge</t>
+          <t>The Irencrag</t>
         </is>
       </c>
       <c r="D924" t="inlineStr"/>
       <c r="E924" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F924" t="b">
@@ -22331,13 +22331,13 @@
       </c>
       <c r="C925" t="inlineStr">
         <is>
-          <t>The Irencrag</t>
+          <t>The Master, Multiplied</t>
         </is>
       </c>
       <c r="D925" t="inlineStr"/>
       <c r="E925" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F925" t="b">
@@ -22353,13 +22353,13 @@
       </c>
       <c r="C926" t="inlineStr">
         <is>
-          <t>The Master, Multiplied</t>
+          <t>The Reaver Cleaver</t>
         </is>
       </c>
       <c r="D926" t="inlineStr"/>
       <c r="E926" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F926" t="b">
@@ -22375,13 +22375,13 @@
       </c>
       <c r="C927" t="inlineStr">
         <is>
-          <t>The Reaver Cleaver</t>
+          <t>The Skullspore Nexus</t>
         </is>
       </c>
       <c r="D927" t="inlineStr"/>
       <c r="E927" t="inlineStr">
         <is>
-          <t>gwyn</t>
+          <t>gishath</t>
         </is>
       </c>
       <c r="F927" t="b">
@@ -22397,13 +22397,13 @@
       </c>
       <c r="C928" t="inlineStr">
         <is>
-          <t>The Skullspore Nexus</t>
+          <t>The Sound of Drums</t>
         </is>
       </c>
       <c r="D928" t="inlineStr"/>
       <c r="E928" t="inlineStr">
         <is>
-          <t>gishath</t>
+          <t>xantcha</t>
         </is>
       </c>
       <c r="F928" t="b">
@@ -22419,13 +22419,13 @@
       </c>
       <c r="C929" t="inlineStr">
         <is>
-          <t>The Sound of Drums</t>
+          <t>Thornwood Falls</t>
         </is>
       </c>
       <c r="D929" t="inlineStr"/>
       <c r="E929" t="inlineStr">
         <is>
-          <t>xantcha</t>
+          <t>arix</t>
         </is>
       </c>
       <c r="F929" t="b">
@@ -22441,13 +22441,13 @@
       </c>
       <c r="C930" t="inlineStr">
         <is>
-          <t>Thornwood Falls</t>
+          <t>Thousand-Faced Shadow</t>
         </is>
       </c>
       <c r="D930" t="inlineStr"/>
       <c r="E930" t="inlineStr">
         <is>
-          <t>arix</t>
+          <t>goro</t>
         </is>
       </c>
       <c r="F930" t="b">
@@ -22463,13 +22463,13 @@
       </c>
       <c r="C931" t="inlineStr">
         <is>
-          <t>Thousand-Faced Shadow</t>
+          <t>Thran Power Suit</t>
         </is>
       </c>
       <c r="D931" t="inlineStr"/>
       <c r="E931" t="inlineStr">
         <is>
-          <t>goro</t>
+          <t>gwyn</t>
         </is>
       </c>
       <c r="F931" t="b">
@@ -22601,7 +22601,7 @@
       <c r="D937" t="inlineStr"/>
       <c r="E937" t="inlineStr">
         <is>
-          <t>temp</t>
+          <t>maja</t>
         </is>
       </c>
       <c r="F937" t="b">

</xml_diff>